<commit_message>
de 25 a 36 preguntas rag
</commit_message>
<xml_diff>
--- a/Local/faqs.xlsx
+++ b/Local/faqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\Tesis\Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8454752F-BE5C-4E20-845A-1188B4D5C8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42311AC9-717A-4A68-9AD2-86384E2C3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>type</t>
   </si>
@@ -354,20 +354,53 @@
     </r>
   </si>
   <si>
-    <t>img</t>
-  </si>
-  <si>
-    <t>¿Cuál es el proceso de inscripción de la Rio21k?</t>
-  </si>
-  <si>
-    <t>imagenes\inscripcion_rio21k.jpg</t>
+    <t>Que hotel recomiendan? (hostal/airbnb)</t>
+  </si>
+  <si>
+    <t>cuales son los horarios de inicio/salida de la carrera</t>
+  </si>
+  <si>
+    <t>Como confirmo la recepcion de mi pago de la inscripcion?</t>
+  </si>
+  <si>
+    <t>como es el proceso de inscripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que incluye mi pago? </t>
+  </si>
+  <si>
+    <t>Información sobre la ruta del hielo/yelero/ielero/hielero</t>
+  </si>
+  <si>
+    <t>desde donde inician las carreras?</t>
+  </si>
+  <si>
+    <t>deseo registrarme en la carrera</t>
+  </si>
+  <si>
+    <t>si somos un grupo de amigos, hay alguna promo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cual es el punto de salida de las carreras? </t>
+  </si>
+  <si>
+    <t>¡Una gran experiencia empieza con un gran lugar para alojarse! El hospedaje oficial del evento es la espectacular Hostería Andaluza, ideal para prepararte con tranquilidad antes del gran día y recargar energías después del desafío. Encuéntralos en Instagram como @hosterialaandaluza. 🏞️🔥</t>
+  </si>
+  <si>
+    <t>si ya hice el pago, debo mandarlo a algun lugar?</t>
+  </si>
+  <si>
+    <t>Hola.La Ruta del Hielero, parte desde la parroquia de San Juan a 25 minutos de Riobamba.
+Tenemos 5 distancias, 5k, 10k, 25k, 40k y 70k.
+Esta carrera está calificada por la ASET, Asociación Ecuatoriana de Trail como evento clasificatorio para la selección nacional de trail, que representará al País en torneos internacionales.
+Además cuenta con INDEX UTMB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +438,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -441,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -455,6 +494,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="C29" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -952,14 +992,124 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C29" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>56</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevo faq 12 oct
</commit_message>
<xml_diff>
--- a/Local/faqs.xlsx
+++ b/Local/faqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\Tesis\Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B7542A-CFB7-41BE-823B-F1FC5F9976D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04757305-5425-4A6A-9871-11EEAFCC233D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
   <si>
     <t>type</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>faq</t>
-  </si>
-  <si>
-    <t>¡Hora de equiparte para el desafío! La entrega de kits será en el concesionario Nissan Renault, de 11h00 a 18h00.
-⚠️ Recuerda que no se entregan kits el día de la carrera bajo ninguna circunstancia.
-🔄 Ten listo tu código QR de confirmación para agilizar el proceso.
-Aquí te dejo la ubicación para que no te pierdas 👉 [link de Google Maps]</t>
   </si>
   <si>
     <t>Más que una inscripción, es tu entrada a una experiencia completa:
@@ -92,9 +86,6 @@
     <t>¿Cuándo inician las inscripciones para la próxima carrera?</t>
   </si>
   <si>
-    <t>Donde se entregarán los kits ?</t>
-  </si>
-  <si>
     <t>¿Me puedo cambiar de distancia?</t>
   </si>
   <si>
@@ -176,17 +167,6 @@
 🌋 Ruta del Hielero y Altar Reto Trail: 5K, 10K, 25K, 40K y 70K
 🌊 Río 21K: 5K, 10K y 21K
 Elige tu desafío y prepárate para conquistarlo 💪🏔️</t>
-  </si>
-  <si>
-    <t>Hola. El Altar Reto Trail se realizará el domingo 21 de septiembre, con punto de partida en la parroquia Quimiag, a 20 minutos de Riobamba.
-Las distancias disponibles son: 5K, 10K, 25K, 40K y 70K.
-Este evento está avalado por ASET como clasificatorio para la selección nacional de trail y cuenta con índice UTMB, válido para competencias internacionales.</t>
-  </si>
-  <si>
-    <t>Hola. El Altar Reto Trail es el (FECHA), parte desde la parroquia de San Juan a 25 minutos de Riobamba.
-Tenemos 5 distancias, 5k, 10k, 25k, 40k y 70k.
-Esta carrera está calificada por la ASET, Asociación Ecuatoriana de Trail como evento clasificatorio para la selección nacional de trail, que representará al País en torneos internacionales.
-Además cuenta con INDEX UTMB</t>
   </si>
   <si>
     <t>La Río 21K es nuestra última gran cita del año, y será el 23 de noviembre.
@@ -395,18 +375,92 @@
 Esta carrera está calificada por la ASET, Asociación Ecuatoriana de Trail como evento clasificatorio para la selección nacional de trail, que representará al País en torneos internacionales.
 Además cuenta con INDEX UTMB</t>
   </si>
+  <si>
+    <t>Una vez que hayas enviado el comprobante de depósito o transferencia vas a recibir un código y link para completar tu registro.</t>
+  </si>
+  <si>
+    <t>¡Hora de equiparte para el desafío! La entrega de kits para Altar Reto Trail será en el concesionario Nissan Renault el 18 de Octubre de 11h00 a 18h00.
+⚠️ Recuerda que no se entregan kits el día de la carrera bajo ninguna circunstancia.
+🔄 Ten listo tu código QR de confirmación para agilizar el proceso.
+Aquí te dejo la ubicación para que no te pierdas 👉 [link de Google Maps]</t>
+  </si>
+  <si>
+    <t>Donde se entregarán los kits (Altar Reto Trail)?</t>
+  </si>
+  <si>
+    <t>Donde se entregarán los kits (Ruta del Hielero)?</t>
+  </si>
+  <si>
+    <t>Donde se entregarán los kits (Rio 21K)?</t>
+  </si>
+  <si>
+    <t>¡Hora de equiparte para el desafío! La entrega de kits para Ruta del Hielero será en el concesionario Nissan Renault el 3 de Mayo de 11h00 a 18h00.
+⚠️ Recuerda que no se entregan kits el día de la carrera bajo ninguna circunstancia.
+🔄 Ten listo tu código QR de confirmación para agilizar el proceso.
+Aquí te dejo la ubicación para que no te pierdas 👉 [link de Google Maps]</t>
+  </si>
+  <si>
+    <t>¡Hora de equiparte para el desafío! La entrega de kits para Rio 21K será en el concesionario Nissan Renault el 21 de Noviembre de 11h00 a 18h00.
+⚠️ Recuerda que no se entregan kits el día de la carrera bajo ninguna circunstancia.
+🔄 Ten listo tu código QR de confirmación para agilizar el proceso.
+Aquí te dejo la ubicación para que no te pierdas 👉 [link de Google Maps]</t>
+  </si>
+  <si>
+    <t>Por qué se cambio de fecha la carrera ?</t>
+  </si>
+  <si>
+    <t>¡Hola! 👋
+La fecha del Altar Reto Trail se cambió por motivos de fuerza mayor relacionados con la situación actual del país y el toque de queda en Chimborazo, que dificultaban la logística y seguridad del evento.
+La nueva fecha es el 19 de octubre, elegida para afectar lo menos posible a nuestra comunidad de corredores 🏔️</t>
+  </si>
+  <si>
+    <t>Ya tengo el código para completar mi inscripción, qué sigue?</t>
+  </si>
+  <si>
+    <t>Por favor para completar tu inscripción y llenar tus datos finales, sigue el siguiente link : https://naftaecplus.com/carreras/</t>
+  </si>
+  <si>
+    <t>No me llega el código de confirmación, qué puedo hacer?</t>
+  </si>
+  <si>
+    <t>Si es que ya han pasado 48 horas y no recibes tu código para seguir tu inscripción, por favor comunicate al siguiente número +593 99 423 9837</t>
+  </si>
+  <si>
+    <t>Si, para completar tu inscripción envía tu comprobante de pago por Whatsapp y en 48 horas recibirás un código único  y link para completar tu inscripción</t>
+  </si>
+  <si>
+    <t>Te comparto los pasos para que formes parte de esta aventura! 1. Realiza tu depósito o transferencia para confirmar tu cupo 2. Envía el comprobante de pago por este medio 3. En 48 horas recibirás un código y link para completar tu registro y listo!</t>
+  </si>
+  <si>
+    <t>Hola. El Altar Reto Trail se realizará el domingo 19 de Octubre, con punto de partida en la parroquia Quimiag, a 20 minutos de Riobamba.
+Las distancias disponibles son: 5K, 10K, 25K, 40K y 70K.
+Este evento está avalado por ASET como clasificatorio para la selección nacional de trail y cuenta con índice UTMB, válido para competencias internacionales.</t>
+  </si>
+  <si>
+    <t>Hola.La Ruta del Hielero se realizará este 4 de mayo, parte desde la parroquia de San Juan a 25 minutos de Riobamba.
+Tenemos 5 distancias, 5k, 10k, 25k, 40k y 70k.
+Esta carrera está calificada por la ASET, Asociación Ecuatoriana de Trail como evento clasificatorio para la selección nacional de trail, que representará al País en torneos internacionales.
+Además cuenta con INDEX UTMB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -487,23 +541,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="219" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="131" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -731,10 +791,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -742,10 +802,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -753,10 +813,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -764,10 +824,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -775,10 +835,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -786,21 +846,21 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>50</v>
+      <c r="C8" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -808,21 +868,21 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
+      <c r="C10" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -830,10 +890,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -841,21 +901,21 @@
         <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
+      <c r="B13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -863,10 +923,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -874,10 +934,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -885,10 +945,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -896,10 +956,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -907,10 +967,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -918,10 +978,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -929,10 +989,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -940,10 +1000,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -951,10 +1011,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -962,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -973,10 +1033,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -984,10 +1044,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -995,10 +1055,10 @@
         <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1006,10 +1066,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1017,10 +1077,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1028,10 +1088,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1039,10 +1099,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1050,10 +1110,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1061,10 +1121,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1072,10 +1132,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1083,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,21 +1154,19 @@
         <v>3</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1116,10 +1174,65 @@
         <v>3</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>35</v>
+        <v>61</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version with people lookup.
</commit_message>
<xml_diff>
--- a/Local/faqs.xlsx
+++ b/Local/faqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\Tesis\Local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E32163A-C483-4E45-A70A-787DAA00BD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5FD39B-077F-4887-86BC-1F9BB9721994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>type</t>
   </si>
@@ -570,18 +570,31 @@
   <si>
     <t>NAFTAEC organiza 3 carreras, las cuales son: Ruta del Hielero, Altar Reto Trail y Rio 21K</t>
   </si>
+  <si>
+    <t>Tienen descuentos?</t>
+  </si>
+  <si>
+    <t>Dame precios de las carreras</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -683,35 +696,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="131" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="131" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1473,6 +1492,28 @@
         <v>93</v>
       </c>
     </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>